<commit_message>
Predicting for several weeks ahead
</commit_message>
<xml_diff>
--- a/train_results/on-trade_train_result.xlsx
+++ b/train_results/on-trade_train_result.xlsx
@@ -594,7 +594,7 @@
         <v>145</v>
       </c>
       <c r="T2" t="n">
-        <v>378</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3">
@@ -652,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -716,7 +716,7 @@
         <v>736</v>
       </c>
       <c r="T4" t="n">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="5">
@@ -844,7 +844,7 @@
         <v>1363</v>
       </c>
       <c r="T6" t="n">
-        <v>1563</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="7">
@@ -908,7 +908,7 @@
         <v>247.75</v>
       </c>
       <c r="T7" t="n">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8">
@@ -972,7 +972,7 @@
         <v>1745</v>
       </c>
       <c r="T8" t="n">
-        <v>2645</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="9">
@@ -1036,7 +1036,7 @@
         <v>361.25</v>
       </c>
       <c r="T9" t="n">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10">
@@ -1216,7 +1216,7 @@
         <v>113.125</v>
       </c>
       <c r="T12" t="n">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13">
@@ -1280,7 +1280,7 @@
         <v>210.25</v>
       </c>
       <c r="T13" t="n">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14">
@@ -1338,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="T14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -1464,7 +1464,7 @@
         <v>12.078125</v>
       </c>
       <c r="T16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -1528,7 +1528,7 @@
         <v>154</v>
       </c>
       <c r="T17" t="n">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18">
@@ -1586,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="T18" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -1708,7 +1708,7 @@
         <v>364</v>
       </c>
       <c r="T20" t="n">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21">
@@ -1772,7 +1772,7 @@
         <v>65</v>
       </c>
       <c r="T21" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22">
@@ -1836,7 +1836,7 @@
         <v>879.5</v>
       </c>
       <c r="T22" t="n">
-        <v>1229</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="23">
@@ -1900,7 +1900,7 @@
         <v>136.5</v>
       </c>
       <c r="T23" t="n">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24">
@@ -2150,7 +2150,7 @@
         <v>0</v>
       </c>
       <c r="T27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
@@ -2278,7 +2278,7 @@
         <v>277.25</v>
       </c>
       <c r="T29" t="n">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30">
@@ -2468,7 +2468,7 @@
         <v>8.25</v>
       </c>
       <c r="T32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -2644,7 +2644,7 @@
         <v>0</v>
       </c>
       <c r="T35" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36">
@@ -2766,7 +2766,7 @@
         <v>461</v>
       </c>
       <c r="T37" t="n">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="38">
@@ -2830,7 +2830,7 @@
         <v>569.5</v>
       </c>
       <c r="T38" t="n">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="39">
@@ -2958,7 +2958,7 @@
         <v>964</v>
       </c>
       <c r="T40" t="n">
-        <v>1575</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="41">
@@ -3022,7 +3022,7 @@
         <v>90</v>
       </c>
       <c r="T41" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42">
@@ -3206,7 +3206,7 @@
         <v>482.5</v>
       </c>
       <c r="T44" t="n">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="45">
@@ -3334,7 +3334,7 @@
         <v>580.5</v>
       </c>
       <c r="T46" t="n">
-        <v>1168</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="47">
@@ -3398,7 +3398,7 @@
         <v>192.5</v>
       </c>
       <c r="T47" t="n">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48">
@@ -4022,7 +4022,7 @@
         <v>128.625</v>
       </c>
       <c r="T57" t="n">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58">
@@ -4086,7 +4086,7 @@
         <v>8.015625</v>
       </c>
       <c r="T58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59">
@@ -4150,7 +4150,7 @@
         <v>190.125</v>
       </c>
       <c r="T59" t="n">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="60">
@@ -4580,7 +4580,7 @@
         <v>509.5</v>
       </c>
       <c r="T66" t="n">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="67">
@@ -4708,7 +4708,7 @@
         <v>892</v>
       </c>
       <c r="T68" t="n">
-        <v>1502</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="69">
@@ -4772,7 +4772,7 @@
         <v>19</v>
       </c>
       <c r="T69" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70">
@@ -5570,7 +5570,7 @@
         <v>14</v>
       </c>
       <c r="T82" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83">
@@ -5632,7 +5632,7 @@
         <v>9.6015625</v>
       </c>
       <c r="T83" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="84">
@@ -5942,7 +5942,7 @@
         <v>9.8515625</v>
       </c>
       <c r="T88" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="89">
@@ -6064,7 +6064,7 @@
         <v>220</v>
       </c>
       <c r="T90" t="n">
-        <v>456</v>
+        <v>467</v>
       </c>
     </row>
     <row r="91">
@@ -6124,7 +6124,7 @@
         <v>0</v>
       </c>
       <c r="T91" t="n">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="92">
@@ -6188,7 +6188,7 @@
         <v>988.5</v>
       </c>
       <c r="T92" t="n">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="93">
@@ -6316,7 +6316,7 @@
         <v>2550</v>
       </c>
       <c r="T94" t="n">
-        <v>1498</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="95">
@@ -6380,7 +6380,7 @@
         <v>278</v>
       </c>
       <c r="T95" t="n">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="96">
@@ -6444,7 +6444,7 @@
         <v>3060</v>
       </c>
       <c r="T96" t="n">
-        <v>2799</v>
+        <v>2797</v>
       </c>
     </row>
     <row r="97">
@@ -6508,7 +6508,7 @@
         <v>386.25</v>
       </c>
       <c r="T97" t="n">
-        <v>372</v>
+        <v>376</v>
       </c>
     </row>
     <row r="98">
@@ -6566,7 +6566,7 @@
         <v>0</v>
       </c>
       <c r="T98" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99">
@@ -6624,7 +6624,7 @@
         <v>0</v>
       </c>
       <c r="T99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -6752,7 +6752,7 @@
         <v>336.25</v>
       </c>
       <c r="T101" t="n">
-        <v>356</v>
+        <v>361</v>
       </c>
     </row>
     <row r="102">
@@ -6810,7 +6810,7 @@
         <v>0</v>
       </c>
       <c r="T102" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103">
@@ -7002,7 +7002,7 @@
         <v>249.375</v>
       </c>
       <c r="T105" t="n">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="106">
@@ -7246,7 +7246,7 @@
         <v>62.6875</v>
       </c>
       <c r="T109" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="110">
@@ -7310,7 +7310,7 @@
         <v>1479</v>
       </c>
       <c r="T110" t="n">
-        <v>1297</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="111">
@@ -7374,7 +7374,7 @@
         <v>140.75</v>
       </c>
       <c r="T111" t="n">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="112">
@@ -7438,7 +7438,7 @@
         <v>167.25</v>
       </c>
       <c r="T112" t="n">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="113">
@@ -7566,7 +7566,7 @@
         <v>123</v>
       </c>
       <c r="T114" t="n">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="115">
@@ -7624,7 +7624,7 @@
         <v>0</v>
       </c>
       <c r="T115" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116">
@@ -7752,7 +7752,7 @@
         <v>261.25</v>
       </c>
       <c r="T117" t="n">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="118">
@@ -7816,7 +7816,7 @@
         <v>51.3125</v>
       </c>
       <c r="T118" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="119">
@@ -7880,7 +7880,7 @@
         <v>39.75</v>
       </c>
       <c r="T119" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="120">
@@ -8058,7 +8058,7 @@
         <v>0</v>
       </c>
       <c r="T122" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123">
@@ -8120,7 +8120,7 @@
         <v>0</v>
       </c>
       <c r="T123" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="124">
@@ -8242,7 +8242,7 @@
         <v>652</v>
       </c>
       <c r="T125" t="n">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="126">
@@ -8306,7 +8306,7 @@
         <v>847</v>
       </c>
       <c r="T126" t="n">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="127">
@@ -8434,7 +8434,7 @@
         <v>1854</v>
       </c>
       <c r="T128" t="n">
-        <v>1410</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="129">
@@ -8682,7 +8682,7 @@
         <v>800.5</v>
       </c>
       <c r="T132" t="n">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="133">
@@ -8810,7 +8810,7 @@
         <v>1166</v>
       </c>
       <c r="T134" t="n">
-        <v>1175</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="135">
@@ -8874,7 +8874,7 @@
         <v>187</v>
       </c>
       <c r="T135" t="n">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="136">
@@ -9066,7 +9066,7 @@
         <v>18</v>
       </c>
       <c r="T138" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="139">
@@ -9190,7 +9190,7 @@
         <v>65.0625</v>
       </c>
       <c r="T140" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="141">
@@ -9552,7 +9552,7 @@
         <v>189.25</v>
       </c>
       <c r="T146" t="n">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="147">
@@ -9988,7 +9988,7 @@
         <v>0</v>
       </c>
       <c r="T153" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="154">
@@ -10046,7 +10046,7 @@
         <v>0</v>
       </c>
       <c r="T154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155">
@@ -10110,7 +10110,7 @@
         <v>812.5</v>
       </c>
       <c r="T155" t="n">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="156">
@@ -10174,7 +10174,7 @@
         <v>9.984375</v>
       </c>
       <c r="T156" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="157">
@@ -10238,7 +10238,7 @@
         <v>1586</v>
       </c>
       <c r="T157" t="n">
-        <v>1626</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="158">
@@ -11104,7 +11104,7 @@
         <v>40.5</v>
       </c>
       <c r="T171" t="n">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="172">
@@ -11550,7 +11550,7 @@
         <v>290</v>
       </c>
       <c r="T178" t="n">
-        <v>566</v>
+        <v>570</v>
       </c>
     </row>
     <row r="179">
@@ -11612,7 +11612,7 @@
         <v>100</v>
       </c>
       <c r="T179" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="180">
@@ -11676,7 +11676,7 @@
         <v>1210</v>
       </c>
       <c r="T180" t="n">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="181">
@@ -11740,7 +11740,7 @@
         <v>41.1875</v>
       </c>
       <c r="T181" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="182">
@@ -11804,7 +11804,7 @@
         <v>3658</v>
       </c>
       <c r="T182" t="n">
-        <v>1738</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="183">
@@ -11868,7 +11868,7 @@
         <v>240.75</v>
       </c>
       <c r="T183" t="n">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="184">
@@ -11932,7 +11932,7 @@
         <v>4804</v>
       </c>
       <c r="T184" t="n">
-        <v>3059</v>
+        <v>3030</v>
       </c>
     </row>
     <row r="185">
@@ -11996,7 +11996,7 @@
         <v>399.75</v>
       </c>
       <c r="T185" t="n">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="186">
@@ -12054,7 +12054,7 @@
         <v>0</v>
       </c>
       <c r="T186" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="187">
@@ -12112,7 +12112,7 @@
         <v>0</v>
       </c>
       <c r="T187" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="188">
@@ -12176,7 +12176,7 @@
         <v>250.125</v>
       </c>
       <c r="T188" t="n">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="189">
@@ -12240,7 +12240,7 @@
         <v>719</v>
       </c>
       <c r="T189" t="n">
-        <v>333</v>
+        <v>340</v>
       </c>
     </row>
     <row r="190">
@@ -12362,7 +12362,7 @@
         <v>175.875</v>
       </c>
       <c r="T191" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="192">
@@ -12490,7 +12490,7 @@
         <v>343.75</v>
       </c>
       <c r="T193" t="n">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="194">
@@ -12548,7 +12548,7 @@
         <v>0</v>
       </c>
       <c r="T194" t="n">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="195">
@@ -12670,7 +12670,7 @@
         <v>936</v>
       </c>
       <c r="T196" t="n">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="197">
@@ -12798,7 +12798,7 @@
         <v>2964</v>
       </c>
       <c r="T198" t="n">
-        <v>1477</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="199">
@@ -12862,7 +12862,7 @@
         <v>252.25</v>
       </c>
       <c r="T199" t="n">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="200">
@@ -12926,7 +12926,7 @@
         <v>255.875</v>
       </c>
       <c r="T200" t="n">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="201">
@@ -12990,7 +12990,7 @@
         <v>25.21875</v>
       </c>
       <c r="T201" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="202">
@@ -13054,7 +13054,7 @@
         <v>225.25</v>
       </c>
       <c r="T202" t="n">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="203">
@@ -13112,7 +13112,7 @@
         <v>0</v>
       </c>
       <c r="T203" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="204">
@@ -13240,7 +13240,7 @@
         <v>324.5</v>
       </c>
       <c r="T205" t="n">
-        <v>334</v>
+        <v>327</v>
       </c>
     </row>
     <row r="206">
@@ -13730,7 +13730,7 @@
         <v>902.5</v>
       </c>
       <c r="T213" t="n">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="214">
@@ -13794,7 +13794,7 @@
         <v>1246</v>
       </c>
       <c r="T214" t="n">
-        <v>503</v>
+        <v>492</v>
       </c>
     </row>
     <row r="215">
@@ -13922,7 +13922,7 @@
         <v>2834</v>
       </c>
       <c r="T216" t="n">
-        <v>1597</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="217">
@@ -13986,7 +13986,7 @@
         <v>138.25</v>
       </c>
       <c r="T217" t="n">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="218">
@@ -14106,7 +14106,7 @@
         <v>0</v>
       </c>
       <c r="T219" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="220">
@@ -14170,7 +14170,7 @@
         <v>1100</v>
       </c>
       <c r="T220" t="n">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="221">
@@ -14298,7 +14298,7 @@
         <v>2388</v>
       </c>
       <c r="T222" t="n">
-        <v>1360</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="223">
@@ -14362,7 +14362,7 @@
         <v>390</v>
       </c>
       <c r="T223" t="n">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="224">
@@ -14426,7 +14426,7 @@
         <v>10.484375</v>
       </c>
       <c r="T224" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="225">
@@ -14490,7 +14490,7 @@
         <v>8.1875</v>
       </c>
       <c r="T225" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226">
@@ -14552,7 +14552,7 @@
         <v>28.90625</v>
       </c>
       <c r="T226" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="227">
@@ -14676,7 +14676,7 @@
         <v>82</v>
       </c>
       <c r="T228" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="229">
@@ -14732,7 +14732,7 @@
         <v>100</v>
       </c>
       <c r="T229" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="230">
@@ -14860,7 +14860,7 @@
         <v>32.28125</v>
       </c>
       <c r="T231" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="232">
@@ -15040,7 +15040,7 @@
         <v>289.75</v>
       </c>
       <c r="T234" t="n">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="235">
@@ -15360,7 +15360,7 @@
         <v>20.953125</v>
       </c>
       <c r="T239" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="240">
@@ -15478,7 +15478,7 @@
         <v>0</v>
       </c>
       <c r="T241" t="n">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="242">
@@ -15600,7 +15600,7 @@
         <v>1260</v>
       </c>
       <c r="T243" t="n">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="244">
@@ -15664,7 +15664,7 @@
         <v>12.8125</v>
       </c>
       <c r="T244" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="245">
@@ -15728,7 +15728,7 @@
         <v>2692</v>
       </c>
       <c r="T245" t="n">
-        <v>1984</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="246">
@@ -15982,7 +15982,7 @@
         <v>51.4375</v>
       </c>
       <c r="T249" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="250">
@@ -16158,7 +16158,7 @@
         <v>0</v>
       </c>
       <c r="T252" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="253">
@@ -16286,7 +16286,7 @@
         <v>3.6640625</v>
       </c>
       <c r="T254" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="255">
@@ -16406,7 +16406,7 @@
         <v>0</v>
       </c>
       <c r="T256" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="257">
@@ -16598,7 +16598,7 @@
         <v>58</v>
       </c>
       <c r="T259" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="260">
@@ -16662,7 +16662,7 @@
         <v>123.75</v>
       </c>
       <c r="T260" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="261">
@@ -16898,7 +16898,7 @@
         <v>4.859375</v>
       </c>
       <c r="T264" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="265">
@@ -16962,7 +16962,7 @@
         <v>12.5078125</v>
       </c>
       <c r="T265" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="266">
@@ -17090,7 +17090,7 @@
         <v>100.125</v>
       </c>
       <c r="T267" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="268">
@@ -17152,7 +17152,7 @@
         <v>640</v>
       </c>
       <c r="T268" t="n">
-        <v>739</v>
+        <v>732</v>
       </c>
     </row>
     <row r="269">
@@ -17214,7 +17214,7 @@
         <v>293.25</v>
       </c>
       <c r="T269" t="n">
-        <v>349</v>
+        <v>355</v>
       </c>
     </row>
     <row r="270">
@@ -17278,7 +17278,7 @@
         <v>889</v>
       </c>
       <c r="T270" t="n">
-        <v>1043</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="271">
@@ -17342,7 +17342,7 @@
         <v>170.625</v>
       </c>
       <c r="T271" t="n">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="272">
@@ -17406,7 +17406,7 @@
         <v>2090</v>
       </c>
       <c r="T272" t="n">
-        <v>2689</v>
+        <v>2680</v>
       </c>
     </row>
     <row r="273">
@@ -17470,7 +17470,7 @@
         <v>878</v>
       </c>
       <c r="T273" t="n">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="274">
@@ -17534,7 +17534,7 @@
         <v>3218</v>
       </c>
       <c r="T274" t="n">
-        <v>4872</v>
+        <v>4929</v>
       </c>
     </row>
     <row r="275">
@@ -17598,7 +17598,7 @@
         <v>1200</v>
       </c>
       <c r="T275" t="n">
-        <v>861</v>
+        <v>856</v>
       </c>
     </row>
     <row r="276">
@@ -17714,7 +17714,7 @@
         <v>0</v>
       </c>
       <c r="T277" t="n">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="278">
@@ -17778,7 +17778,7 @@
         <v>167.125</v>
       </c>
       <c r="T278" t="n">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="279">
@@ -17842,7 +17842,7 @@
         <v>488.75</v>
       </c>
       <c r="T279" t="n">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="280">
@@ -17900,7 +17900,7 @@
         <v>0</v>
       </c>
       <c r="T280" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="281">
@@ -18028,7 +18028,7 @@
         <v>38.9375</v>
       </c>
       <c r="T282" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="283">
@@ -18092,7 +18092,7 @@
         <v>338.75</v>
       </c>
       <c r="T283" t="n">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="284">
@@ -18210,7 +18210,7 @@
         <v>100</v>
       </c>
       <c r="T285" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="286">
@@ -18274,7 +18274,7 @@
         <v>427</v>
       </c>
       <c r="T286" t="n">
-        <v>588</v>
+        <v>582</v>
       </c>
     </row>
     <row r="287">
@@ -18402,7 +18402,7 @@
         <v>2066</v>
       </c>
       <c r="T288" t="n">
-        <v>2631</v>
+        <v>2627</v>
       </c>
     </row>
     <row r="289">
@@ -18466,7 +18466,7 @@
         <v>462.25</v>
       </c>
       <c r="T289" t="n">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="290">
@@ -18530,7 +18530,7 @@
         <v>168.875</v>
       </c>
       <c r="T290" t="n">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="291">
@@ -18658,7 +18658,7 @@
         <v>216.25</v>
       </c>
       <c r="T292" t="n">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="293">
@@ -18718,7 +18718,7 @@
         <v>150</v>
       </c>
       <c r="T293" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="294">
@@ -18846,7 +18846,7 @@
         <v>925</v>
       </c>
       <c r="T295" t="n">
-        <v>600</v>
+        <v>606</v>
       </c>
     </row>
     <row r="296">
@@ -18910,7 +18910,7 @@
         <v>171.625</v>
       </c>
       <c r="T296" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="297">
@@ -18974,7 +18974,7 @@
         <v>127</v>
       </c>
       <c r="T297" t="n">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="298">
@@ -19154,7 +19154,7 @@
         <v>0</v>
       </c>
       <c r="T300" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="301">
@@ -19218,7 +19218,7 @@
         <v>70</v>
       </c>
       <c r="T301" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="302">
@@ -19278,7 +19278,7 @@
         <v>20</v>
       </c>
       <c r="T302" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="303">
@@ -19406,7 +19406,7 @@
         <v>576.5</v>
       </c>
       <c r="T304" t="n">
-        <v>808</v>
+        <v>804</v>
       </c>
     </row>
     <row r="305">
@@ -19470,7 +19470,7 @@
         <v>93.125</v>
       </c>
       <c r="T305" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="306">
@@ -19534,7 +19534,7 @@
         <v>2006</v>
       </c>
       <c r="T306" t="n">
-        <v>2696</v>
+        <v>2705</v>
       </c>
     </row>
     <row r="307">
@@ -19598,7 +19598,7 @@
         <v>307.75</v>
       </c>
       <c r="T307" t="n">
-        <v>405</v>
+        <v>412</v>
       </c>
     </row>
     <row r="308">
@@ -19660,7 +19660,7 @@
         <v>20</v>
       </c>
       <c r="T308" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="309">
@@ -19720,7 +19720,7 @@
         <v>80</v>
       </c>
       <c r="T309" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="310">
@@ -19784,7 +19784,7 @@
         <v>617.5</v>
       </c>
       <c r="T310" t="n">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="311">
@@ -19912,7 +19912,7 @@
         <v>1639</v>
       </c>
       <c r="T312" t="n">
-        <v>2310</v>
+        <v>2324</v>
       </c>
     </row>
     <row r="313">
@@ -19976,7 +19976,7 @@
         <v>722.5</v>
       </c>
       <c r="T313" t="n">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="314">
@@ -20168,7 +20168,7 @@
         <v>57.53125</v>
       </c>
       <c r="T316" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="317">
@@ -20294,7 +20294,7 @@
         <v>64.75</v>
       </c>
       <c r="T318" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="319">
@@ -20352,7 +20352,7 @@
         <v>70</v>
       </c>
       <c r="T319" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="320">
@@ -20716,7 +20716,7 @@
         <v>173.875</v>
       </c>
       <c r="T325" t="n">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="326">
@@ -20780,7 +20780,7 @@
         <v>26.203125</v>
       </c>
       <c r="T326" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="327">
@@ -20844,7 +20844,7 @@
         <v>435.5</v>
       </c>
       <c r="T327" t="n">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="328">
@@ -20908,7 +20908,7 @@
         <v>95</v>
       </c>
       <c r="T328" t="n">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="329">
@@ -21036,7 +21036,7 @@
         <v>27.859375</v>
       </c>
       <c r="T330" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="331">
@@ -21154,7 +21154,7 @@
         <v>0</v>
       </c>
       <c r="T332" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="333">
@@ -21214,7 +21214,7 @@
         <v>30</v>
       </c>
       <c r="T333" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="334">
@@ -21278,7 +21278,7 @@
         <v>693.5</v>
       </c>
       <c r="T334" t="n">
-        <v>1020</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="335">
@@ -21406,7 +21406,7 @@
         <v>2092</v>
       </c>
       <c r="T336" t="n">
-        <v>3099</v>
+        <v>3087</v>
       </c>
     </row>
     <row r="337">
@@ -21470,7 +21470,7 @@
         <v>61.625</v>
       </c>
       <c r="T337" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="338">
@@ -21662,7 +21662,7 @@
         <v>51.84375</v>
       </c>
       <c r="T340" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="341">
@@ -21902,7 +21902,7 @@
         <v>2.986328125</v>
       </c>
       <c r="T344" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="345">
@@ -22342,7 +22342,7 @@
         <v>29.578125</v>
       </c>
       <c r="T351" t="n">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="352">
@@ -22580,7 +22580,7 @@
         <v>22.765625</v>
       </c>
       <c r="T355" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="356">
@@ -22766,7 +22766,7 @@
         <v>104.5</v>
       </c>
       <c r="T358" t="n">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="359">
@@ -22830,7 +22830,7 @@
         <v>58.09375</v>
       </c>
       <c r="T359" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="360">
@@ -22894,7 +22894,7 @@
         <v>695</v>
       </c>
       <c r="T360" t="n">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="361">
@@ -22958,7 +22958,7 @@
         <v>276</v>
       </c>
       <c r="T361" t="n">
-        <v>465</v>
+        <v>469</v>
       </c>
     </row>
     <row r="362">
@@ -23150,7 +23150,7 @@
         <v>2452</v>
       </c>
       <c r="T364" t="n">
-        <v>2409</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="365">
@@ -23214,7 +23214,7 @@
         <v>703.5</v>
       </c>
       <c r="T365" t="n">
-        <v>597</v>
+        <v>601</v>
       </c>
     </row>
     <row r="366">
@@ -23278,7 +23278,7 @@
         <v>5460</v>
       </c>
       <c r="T366" t="n">
-        <v>5112</v>
+        <v>5171</v>
       </c>
     </row>
     <row r="367">
@@ -23342,7 +23342,7 @@
         <v>1069</v>
       </c>
       <c r="T367" t="n">
-        <v>1298</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="368">
@@ -23400,7 +23400,7 @@
         <v>0</v>
       </c>
       <c r="T368" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="369">
@@ -23460,7 +23460,7 @@
         <v>0</v>
       </c>
       <c r="T369" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="370">
@@ -23588,7 +23588,7 @@
         <v>633</v>
       </c>
       <c r="T371" t="n">
-        <v>762</v>
+        <v>764</v>
       </c>
     </row>
     <row r="372">
@@ -23712,7 +23712,7 @@
         <v>103.4375</v>
       </c>
       <c r="T373" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="374">
@@ -23840,7 +23840,7 @@
         <v>498</v>
       </c>
       <c r="T375" t="n">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="376">
@@ -23900,7 +23900,7 @@
         <v>0</v>
       </c>
       <c r="T376" t="n">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="377">
@@ -24028,7 +24028,7 @@
         <v>487.75</v>
       </c>
       <c r="T378" t="n">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="379">
@@ -24156,7 +24156,7 @@
         <v>2784</v>
       </c>
       <c r="T380" t="n">
-        <v>2417</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="381">
@@ -24220,7 +24220,7 @@
         <v>661</v>
       </c>
       <c r="T381" t="n">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
     <row r="382">
@@ -24284,7 +24284,7 @@
         <v>139</v>
       </c>
       <c r="T382" t="n">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="383">
@@ -24412,7 +24412,7 @@
         <v>183.375</v>
       </c>
       <c r="T384" t="n">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="385">
@@ -24476,7 +24476,7 @@
         <v>189.75</v>
       </c>
       <c r="T385" t="n">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="386">
@@ -24540,7 +24540,7 @@
         <v>81.1875</v>
       </c>
       <c r="T386" t="n">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="387">
@@ -24604,7 +24604,7 @@
         <v>873.5</v>
       </c>
       <c r="T387" t="n">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="388">
@@ -24732,7 +24732,7 @@
         <v>626</v>
       </c>
       <c r="T389" t="n">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="390">
@@ -24912,7 +24912,7 @@
         <v>0</v>
       </c>
       <c r="T392" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="393">
@@ -25030,7 +25030,7 @@
         <v>90</v>
       </c>
       <c r="T394" t="n">
-        <v>293</v>
+        <v>298</v>
       </c>
     </row>
     <row r="395">
@@ -25094,7 +25094,7 @@
         <v>30.828125</v>
       </c>
       <c r="T395" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="396">
@@ -25158,7 +25158,7 @@
         <v>535.5</v>
       </c>
       <c r="T396" t="n">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="397">
@@ -25222,7 +25222,7 @@
         <v>767</v>
       </c>
       <c r="T397" t="n">
-        <v>1003</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="398">
@@ -25286,7 +25286,7 @@
         <v>71</v>
       </c>
       <c r="T398" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="399">
@@ -25350,7 +25350,7 @@
         <v>3224</v>
       </c>
       <c r="T399" t="n">
-        <v>3096</v>
+        <v>3115</v>
       </c>
     </row>
     <row r="400">
@@ -25414,7 +25414,7 @@
         <v>388</v>
       </c>
       <c r="T400" t="n">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="401">
@@ -25478,7 +25478,7 @@
         <v>20</v>
       </c>
       <c r="T401" t="n">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="402">
@@ -25542,7 +25542,7 @@
         <v>101.5</v>
       </c>
       <c r="T402" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="403">
@@ -25606,7 +25606,7 @@
         <v>751</v>
       </c>
       <c r="T403" t="n">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="404">
@@ -25734,7 +25734,7 @@
         <v>2670</v>
       </c>
       <c r="T405" t="n">
-        <v>2912</v>
+        <v>2952</v>
       </c>
     </row>
     <row r="406">
@@ -25798,7 +25798,7 @@
         <v>961.5</v>
       </c>
       <c r="T406" t="n">
-        <v>1114</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="407">
@@ -25990,7 +25990,7 @@
         <v>58.375</v>
       </c>
       <c r="T409" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="410">
@@ -26360,7 +26360,7 @@
         <v>0</v>
       </c>
       <c r="T415" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="416">
@@ -26734,7 +26734,7 @@
         <v>155</v>
       </c>
       <c r="T421" t="n">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="422">
@@ -26862,7 +26862,7 @@
         <v>55.5625</v>
       </c>
       <c r="T423" t="n">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="424">
@@ -26920,7 +26920,7 @@
         <v>0</v>
       </c>
       <c r="T424" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="425">
@@ -26984,7 +26984,7 @@
         <v>0</v>
       </c>
       <c r="T425" t="n">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="426">
@@ -27046,7 +27046,7 @@
         <v>43.71875</v>
       </c>
       <c r="T426" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="427">
@@ -27110,7 +27110,7 @@
         <v>763</v>
       </c>
       <c r="T427" t="n">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="428">
@@ -27238,7 +27238,7 @@
         <v>3532</v>
       </c>
       <c r="T429" t="n">
-        <v>3304</v>
+        <v>3316</v>
       </c>
     </row>
     <row r="430">
@@ -27302,7 +27302,7 @@
         <v>155</v>
       </c>
       <c r="T430" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="431">
@@ -27366,7 +27366,7 @@
         <v>168.75</v>
       </c>
       <c r="T431" t="n">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="432">
@@ -27612,7 +27612,7 @@
         <v>0</v>
       </c>
       <c r="T435" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="436">
@@ -27730,7 +27730,7 @@
         <v>9.8671875</v>
       </c>
       <c r="T437" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="438">
@@ -28106,7 +28106,7 @@
         <v>254.375</v>
       </c>
       <c r="T443" t="n">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="444">
@@ -28170,7 +28170,7 @@
         <v>222.625</v>
       </c>
       <c r="T444" t="n">
-        <v>301</v>
+        <v>306</v>
       </c>
     </row>
     <row r="445">
@@ -28464,7 +28464,7 @@
         <v>0</v>
       </c>
       <c r="T449" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="450">
@@ -28656,7 +28656,7 @@
         <v>233</v>
       </c>
       <c r="T452" t="n">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="453">
@@ -28720,7 +28720,7 @@
         <v>1380</v>
       </c>
       <c r="T453" t="n">
-        <v>1354</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="454">
@@ -28784,7 +28784,7 @@
         <v>402.5</v>
       </c>
       <c r="T454" t="n">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="455">
@@ -28848,7 +28848,7 @@
         <v>1015</v>
       </c>
       <c r="T455" t="n">
-        <v>875</v>
+        <v>868</v>
       </c>
     </row>
     <row r="456">
@@ -28976,7 +28976,7 @@
         <v>3360</v>
       </c>
       <c r="T457" t="n">
-        <v>2420</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="458">
@@ -29040,7 +29040,7 @@
         <v>688.5</v>
       </c>
       <c r="T458" t="n">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="459">
@@ -29104,7 +29104,7 @@
         <v>7260</v>
       </c>
       <c r="T459" t="n">
-        <v>5890</v>
+        <v>5886</v>
       </c>
     </row>
     <row r="460">
@@ -29168,7 +29168,7 @@
         <v>1201</v>
       </c>
       <c r="T460" t="n">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="461">
@@ -29226,7 +29226,7 @@
         <v>53.21875</v>
       </c>
       <c r="T461" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="462">
@@ -29352,7 +29352,7 @@
         <v>345.75</v>
       </c>
       <c r="T463" t="n">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="464">
@@ -29416,7 +29416,7 @@
         <v>1184</v>
       </c>
       <c r="T464" t="n">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="465">
@@ -29478,7 +29478,7 @@
         <v>123.25</v>
       </c>
       <c r="T465" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="466">
@@ -29670,7 +29670,7 @@
         <v>678.5</v>
       </c>
       <c r="T468" t="n">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="469">
@@ -29732,7 +29732,7 @@
         <v>532.5</v>
       </c>
       <c r="T469" t="n">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="470">
@@ -29796,7 +29796,7 @@
         <v>126.5</v>
       </c>
       <c r="T470" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="471">
@@ -29924,7 +29924,7 @@
         <v>112.75</v>
       </c>
       <c r="T472" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="473">
@@ -29988,7 +29988,7 @@
         <v>4712</v>
       </c>
       <c r="T473" t="n">
-        <v>3090</v>
+        <v>3078</v>
       </c>
     </row>
     <row r="474">
@@ -30244,7 +30244,7 @@
         <v>348</v>
       </c>
       <c r="T477" t="n">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="478">
@@ -30308,7 +30308,7 @@
         <v>195.875</v>
       </c>
       <c r="T478" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="479">
@@ -30436,7 +30436,7 @@
         <v>863</v>
       </c>
       <c r="T480" t="n">
-        <v>654</v>
+        <v>663</v>
       </c>
     </row>
     <row r="481">
@@ -30500,7 +30500,7 @@
         <v>122</v>
       </c>
       <c r="T481" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="482">
@@ -30564,7 +30564,7 @@
         <v>615</v>
       </c>
       <c r="T482" t="n">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="483">
@@ -30628,7 +30628,7 @@
         <v>19.953125</v>
       </c>
       <c r="T483" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="484">
@@ -30808,7 +30808,7 @@
         <v>492</v>
       </c>
       <c r="T486" t="n">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="487">
@@ -31000,7 +31000,7 @@
         <v>872.5</v>
       </c>
       <c r="T489" t="n">
-        <v>799</v>
+        <v>796</v>
       </c>
     </row>
     <row r="490">
@@ -31064,7 +31064,7 @@
         <v>69</v>
       </c>
       <c r="T490" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="491">
@@ -31128,7 +31128,7 @@
         <v>4108</v>
       </c>
       <c r="T491" t="n">
-        <v>2979</v>
+        <v>2999</v>
       </c>
     </row>
     <row r="492">
@@ -31192,7 +31192,7 @@
         <v>413.75</v>
       </c>
       <c r="T492" t="n">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="493">
@@ -31320,7 +31320,7 @@
         <v>68.5</v>
       </c>
       <c r="T494" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="495">
@@ -31384,7 +31384,7 @@
         <v>834.5</v>
       </c>
       <c r="T495" t="n">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="496">
@@ -31448,7 +31448,7 @@
         <v>88</v>
       </c>
       <c r="T496" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="497">
@@ -31512,7 +31512,7 @@
         <v>4680</v>
       </c>
       <c r="T497" t="n">
-        <v>3544</v>
+        <v>3546</v>
       </c>
     </row>
     <row r="498">
@@ -31576,7 +31576,7 @@
         <v>1061</v>
       </c>
       <c r="T498" t="n">
-        <v>937</v>
+        <v>926</v>
       </c>
     </row>
     <row r="499">
@@ -31640,7 +31640,7 @@
         <v>31.265625</v>
       </c>
       <c r="T499" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="500">
@@ -31832,7 +31832,7 @@
         <v>44.59375</v>
       </c>
       <c r="T502" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="503">
@@ -31894,7 +31894,7 @@
         <v>276.5</v>
       </c>
       <c r="T503" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="504">
@@ -32006,7 +32006,7 @@
         <v>0</v>
       </c>
       <c r="T505" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="506">
@@ -32134,7 +32134,7 @@
         <v>87.125</v>
       </c>
       <c r="T507" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="508">
@@ -32376,7 +32376,7 @@
         <v>218.75</v>
       </c>
       <c r="T511" t="n">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="512">
@@ -32504,7 +32504,7 @@
         <v>1019</v>
       </c>
       <c r="T513" t="n">
-        <v>569</v>
+        <v>562</v>
       </c>
     </row>
     <row r="514">
@@ -32632,7 +32632,7 @@
         <v>38.125</v>
       </c>
       <c r="T515" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="516">
@@ -32696,7 +32696,7 @@
         <v>156.5</v>
       </c>
       <c r="T516" t="n">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="517">
@@ -32818,7 +32818,7 @@
         <v>352</v>
       </c>
       <c r="T518" t="n">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="519">
@@ -32946,7 +32946,7 @@
         <v>1139</v>
       </c>
       <c r="T520" t="n">
-        <v>945</v>
+        <v>936</v>
       </c>
     </row>
     <row r="521">
@@ -33074,7 +33074,7 @@
         <v>5632</v>
       </c>
       <c r="T522" t="n">
-        <v>4269</v>
+        <v>4272</v>
       </c>
     </row>
     <row r="523">
@@ -33138,7 +33138,7 @@
         <v>168</v>
       </c>
       <c r="T523" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="524">
@@ -33202,7 +33202,7 @@
         <v>180.125</v>
       </c>
       <c r="T524" t="n">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="525">
@@ -33266,7 +33266,7 @@
         <v>57.15625</v>
       </c>
       <c r="T525" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="526">
@@ -33394,7 +33394,7 @@
         <v>23</v>
       </c>
       <c r="T527" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="528">
@@ -33760,7 +33760,7 @@
         <v>93.75</v>
       </c>
       <c r="T533" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="534">
@@ -33824,7 +33824,7 @@
         <v>38.90625</v>
       </c>
       <c r="T534" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="535">
@@ -33888,7 +33888,7 @@
         <v>502.5</v>
       </c>
       <c r="T535" t="n">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="536">
@@ -33952,7 +33952,7 @@
         <v>306</v>
       </c>
       <c r="T536" t="n">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="537">
@@ -34126,7 +34126,7 @@
         <v>30.4375</v>
       </c>
       <c r="T539" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="540">
@@ -34190,7 +34190,7 @@
         <v>57.6875</v>
       </c>
       <c r="T540" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="541">
@@ -34310,7 +34310,7 @@
         <v>95</v>
       </c>
       <c r="T542" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="543">
@@ -34374,7 +34374,7 @@
         <v>225.375</v>
       </c>
       <c r="T543" t="n">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="544">
@@ -34438,7 +34438,7 @@
         <v>288</v>
       </c>
       <c r="T544" t="n">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="545">
@@ -34502,7 +34502,7 @@
         <v>2418</v>
       </c>
       <c r="T545" t="n">
-        <v>1778</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="546">
@@ -34630,7 +34630,7 @@
         <v>971.5</v>
       </c>
       <c r="T547" t="n">
-        <v>965</v>
+        <v>959</v>
       </c>
     </row>
     <row r="548">
@@ -34758,7 +34758,7 @@
         <v>3492</v>
       </c>
       <c r="T549" t="n">
-        <v>3158</v>
+        <v>3162</v>
       </c>
     </row>
     <row r="550">
@@ -34822,7 +34822,7 @@
         <v>729</v>
       </c>
       <c r="T550" t="n">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="551">
@@ -34886,7 +34886,7 @@
         <v>8108</v>
       </c>
       <c r="T551" t="n">
-        <v>7425</v>
+        <v>7430</v>
       </c>
     </row>
     <row r="552">
@@ -34950,7 +34950,7 @@
         <v>1168</v>
       </c>
       <c r="T552" t="n">
-        <v>1133</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="553">
@@ -35008,7 +35008,7 @@
         <v>0</v>
       </c>
       <c r="T553" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="554">
@@ -35126,7 +35126,7 @@
         <v>0</v>
       </c>
       <c r="T555" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="556">
@@ -35254,7 +35254,7 @@
         <v>2033</v>
       </c>
       <c r="T557" t="n">
-        <v>1277</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="558">
@@ -35382,7 +35382,7 @@
         <v>131.875</v>
       </c>
       <c r="T559" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="560">
@@ -35446,7 +35446,7 @@
         <v>28.53125</v>
       </c>
       <c r="T560" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="561">
@@ -35510,7 +35510,7 @@
         <v>775.5</v>
       </c>
       <c r="T561" t="n">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="562">
@@ -35574,7 +35574,7 @@
         <v>814</v>
       </c>
       <c r="T562" t="n">
-        <v>497</v>
+        <v>491</v>
       </c>
     </row>
     <row r="563">
@@ -35702,7 +35702,7 @@
         <v>731</v>
       </c>
       <c r="T564" t="n">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="565">
@@ -35830,7 +35830,7 @@
         <v>5784</v>
       </c>
       <c r="T566" t="n">
-        <v>3844</v>
+        <v>3839</v>
       </c>
     </row>
     <row r="567">
@@ -35894,7 +35894,7 @@
         <v>686.5</v>
       </c>
       <c r="T567" t="n">
-        <v>635</v>
+        <v>638</v>
       </c>
     </row>
     <row r="568">
@@ -35958,7 +35958,7 @@
         <v>206.875</v>
       </c>
       <c r="T568" t="n">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="569">
@@ -36086,7 +36086,7 @@
         <v>451.5</v>
       </c>
       <c r="T570" t="n">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="571">
@@ -36460,7 +36460,7 @@
         <v>638</v>
       </c>
       <c r="T576" t="n">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="577">
@@ -36640,7 +36640,7 @@
         <v>0</v>
       </c>
       <c r="T579" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="580">
@@ -36704,7 +36704,7 @@
         <v>687.5</v>
       </c>
       <c r="T580" t="n">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="581">
@@ -36832,7 +36832,7 @@
         <v>552.5</v>
       </c>
       <c r="T582" t="n">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="583">
@@ -36896,7 +36896,7 @@
         <v>980</v>
       </c>
       <c r="T583" t="n">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="584">
@@ -37024,7 +37024,7 @@
         <v>4840</v>
       </c>
       <c r="T585" t="n">
-        <v>3978</v>
+        <v>3975</v>
       </c>
     </row>
     <row r="586">
@@ -37088,7 +37088,7 @@
         <v>374.25</v>
       </c>
       <c r="T586" t="n">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="587">
@@ -37280,7 +37280,7 @@
         <v>912</v>
       </c>
       <c r="T589" t="n">
-        <v>876</v>
+        <v>877</v>
       </c>
     </row>
     <row r="590">
@@ -37408,7 +37408,7 @@
         <v>5432</v>
       </c>
       <c r="T591" t="n">
-        <v>4323</v>
+        <v>4329</v>
       </c>
     </row>
     <row r="592">
@@ -37472,7 +37472,7 @@
         <v>1104</v>
       </c>
       <c r="T592" t="n">
-        <v>981</v>
+        <v>983</v>
       </c>
     </row>
     <row r="593">
@@ -37664,7 +37664,7 @@
         <v>264.75</v>
       </c>
       <c r="T595" t="n">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="596">
@@ -37902,7 +37902,7 @@
         <v>0</v>
       </c>
       <c r="T599" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="600">
@@ -38086,7 +38086,7 @@
         <v>122.9375</v>
       </c>
       <c r="T602" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="603">
@@ -38454,7 +38454,7 @@
         <v>1287</v>
       </c>
       <c r="T608" t="n">
-        <v>736</v>
+        <v>740</v>
       </c>
     </row>
     <row r="609">
@@ -38886,7 +38886,7 @@
         <v>0</v>
       </c>
       <c r="T615" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="616">
@@ -38950,7 +38950,7 @@
         <v>1240</v>
       </c>
       <c r="T616" t="n">
-        <v>1064</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="617">
@@ -39078,7 +39078,7 @@
         <v>7472</v>
       </c>
       <c r="T618" t="n">
-        <v>4769</v>
+        <v>4754</v>
       </c>
     </row>
     <row r="619">
@@ -39142,7 +39142,7 @@
         <v>181</v>
       </c>
       <c r="T619" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="620">
@@ -39206,7 +39206,7 @@
         <v>175.5</v>
       </c>
       <c r="T620" t="n">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="621">
@@ -39334,7 +39334,7 @@
         <v>121</v>
       </c>
       <c r="T622" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="623">
@@ -39570,7 +39570,7 @@
         <v>25.578125</v>
       </c>
       <c r="T626" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="627">
@@ -39946,7 +39946,7 @@
         <v>814.5</v>
       </c>
       <c r="T632" t="n">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="633">
@@ -40564,7 +40564,7 @@
         <v>2650</v>
       </c>
       <c r="T642" t="n">
-        <v>2141</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="643">
@@ -40692,7 +40692,7 @@
         <v>849</v>
       </c>
       <c r="T644" t="n">
-        <v>1008</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="645">
@@ -40820,7 +40820,7 @@
         <v>3226</v>
       </c>
       <c r="T646" t="n">
-        <v>3453</v>
+        <v>3454</v>
       </c>
     </row>
     <row r="647">
@@ -40884,7 +40884,7 @@
         <v>734</v>
       </c>
       <c r="T647" t="n">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="648">
@@ -40948,7 +40948,7 @@
         <v>8044</v>
       </c>
       <c r="T648" t="n">
-        <v>8608</v>
+        <v>8622</v>
       </c>
     </row>
     <row r="649">
@@ -41012,7 +41012,7 @@
         <v>1195</v>
       </c>
       <c r="T649" t="n">
-        <v>1266</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="650">
@@ -41134,7 +41134,7 @@
         <v>216.25</v>
       </c>
       <c r="T651" t="n">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="652">
@@ -41318,7 +41318,7 @@
         <v>1762</v>
       </c>
       <c r="T654" t="n">
-        <v>1492</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="655">
@@ -41574,7 +41574,7 @@
         <v>638.5</v>
       </c>
       <c r="T658" t="n">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="659">
@@ -41638,7 +41638,7 @@
         <v>879</v>
       </c>
       <c r="T659" t="n">
-        <v>521</v>
+        <v>513</v>
       </c>
     </row>
     <row r="660">
@@ -41766,7 +41766,7 @@
         <v>593</v>
       </c>
       <c r="T661" t="n">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="662">
@@ -41894,7 +41894,7 @@
         <v>4996</v>
       </c>
       <c r="T663" t="n">
-        <v>4370</v>
+        <v>4382</v>
       </c>
     </row>
     <row r="664">
@@ -41958,7 +41958,7 @@
         <v>824.5</v>
       </c>
       <c r="T664" t="n">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="665">
@@ -42150,7 +42150,7 @@
         <v>374.25</v>
       </c>
       <c r="T667" t="n">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="668">
@@ -42398,7 +42398,7 @@
         <v>925</v>
       </c>
       <c r="T671" t="n">
-        <v>897</v>
+        <v>894</v>
       </c>
     </row>
     <row r="672">
@@ -42526,7 +42526,7 @@
         <v>605</v>
       </c>
       <c r="T673" t="n">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="674">
@@ -42590,7 +42590,7 @@
         <v>28.453125</v>
       </c>
       <c r="T674" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="675">
@@ -42898,7 +42898,7 @@
         <v>422.25</v>
       </c>
       <c r="T679" t="n">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="680">
@@ -43016,7 +43016,7 @@
         <v>845.5</v>
       </c>
       <c r="T681" t="n">
-        <v>1025</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="682">
@@ -43080,7 +43080,7 @@
         <v>62.375</v>
       </c>
       <c r="T682" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="683">
@@ -43144,7 +43144,7 @@
         <v>4376</v>
       </c>
       <c r="T683" t="n">
-        <v>4590</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="684">
@@ -43208,7 +43208,7 @@
         <v>443.75</v>
       </c>
       <c r="T684" t="n">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="685">
@@ -43400,7 +43400,7 @@
         <v>792</v>
       </c>
       <c r="T687" t="n">
-        <v>986</v>
+        <v>987</v>
       </c>
     </row>
     <row r="688">
@@ -43528,7 +43528,7 @@
         <v>5044</v>
       </c>
       <c r="T689" t="n">
-        <v>4958</v>
+        <v>4975</v>
       </c>
     </row>
     <row r="690">
@@ -43592,7 +43592,7 @@
         <v>1138</v>
       </c>
       <c r="T690" t="n">
-        <v>1204</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="691">
@@ -43720,7 +43720,7 @@
         <v>19.203125</v>
       </c>
       <c r="T692" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="693">
@@ -43784,7 +43784,7 @@
         <v>499.75</v>
       </c>
       <c r="T693" t="n">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="694">
@@ -43910,7 +43910,7 @@
         <v>342.5</v>
       </c>
       <c r="T695" t="n">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="696">
@@ -43968,7 +43968,7 @@
         <v>0</v>
       </c>
       <c r="T696" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="697">
@@ -44026,7 +44026,7 @@
         <v>200</v>
       </c>
       <c r="T697" t="n">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="698">
@@ -44154,7 +44154,7 @@
         <v>116.875</v>
       </c>
       <c r="T699" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="700">
@@ -44272,7 +44272,7 @@
         <v>0</v>
       </c>
       <c r="T701" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="702">
@@ -44398,7 +44398,7 @@
         <v>200.75</v>
       </c>
       <c r="T703" t="n">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="704">
@@ -44526,7 +44526,7 @@
         <v>1046</v>
       </c>
       <c r="T705" t="n">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="706">
@@ -44654,7 +44654,7 @@
         <v>34.125</v>
       </c>
       <c r="T707" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="708">
@@ -44718,7 +44718,7 @@
         <v>209.375</v>
       </c>
       <c r="T708" t="n">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="709">
@@ -44842,7 +44842,7 @@
         <v>682</v>
       </c>
       <c r="T710" t="n">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="711">
@@ -44962,7 +44962,7 @@
         <v>142.75</v>
       </c>
       <c r="T712" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="713">
@@ -45154,7 +45154,7 @@
         <v>6312</v>
       </c>
       <c r="T715" t="n">
-        <v>5749</v>
+        <v>5761</v>
       </c>
     </row>
     <row r="716">
@@ -45410,7 +45410,7 @@
         <v>130</v>
       </c>
       <c r="T719" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="720">
@@ -45474,7 +45474,7 @@
         <v>26</v>
       </c>
       <c r="T720" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="721">
@@ -45528,7 +45528,7 @@
         <v>0</v>
       </c>
       <c r="T721" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="722">
@@ -45592,7 +45592,7 @@
         <v>19.265625</v>
       </c>
       <c r="T722" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="723">
@@ -45720,7 +45720,7 @@
         <v>11</v>
       </c>
       <c r="T724" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="725">
@@ -45776,7 +45776,7 @@
         <v>0</v>
       </c>
       <c r="T725" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="726">
@@ -45968,7 +45968,7 @@
         <v>1044</v>
       </c>
       <c r="T728" t="n">
-        <v>1058</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="729">
@@ -46032,7 +46032,7 @@
         <v>391</v>
       </c>
       <c r="T729" t="n">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="730">
@@ -46090,7 +46090,7 @@
         <v>180</v>
       </c>
       <c r="T730" t="n">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="731">
@@ -46150,7 +46150,7 @@
         <v>0</v>
       </c>
       <c r="T731" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="732">
@@ -46214,7 +46214,7 @@
         <v>46.90625</v>
       </c>
       <c r="T732" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="733">
@@ -46278,7 +46278,7 @@
         <v>138.625</v>
       </c>
       <c r="T733" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="734">
@@ -46398,7 +46398,7 @@
         <v>165.125</v>
       </c>
       <c r="T735" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="736">
@@ -46462,7 +46462,7 @@
         <v>451</v>
       </c>
       <c r="T736" t="n">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="737">
@@ -46526,7 +46526,7 @@
         <v>386</v>
       </c>
       <c r="T737" t="n">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="738">
@@ -46590,7 +46590,7 @@
         <v>2674</v>
       </c>
       <c r="T738" t="n">
-        <v>2649</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="739">
@@ -46654,7 +46654,7 @@
         <v>374.5</v>
       </c>
       <c r="T739" t="n">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="740">
@@ -46708,7 +46708,7 @@
         <v>1.349609375</v>
       </c>
       <c r="T740" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="741">
@@ -46826,7 +46826,7 @@
         <v>848</v>
       </c>
       <c r="T742" t="n">
-        <v>1182</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="743">
@@ -46954,7 +46954,7 @@
         <v>3806</v>
       </c>
       <c r="T744" t="n">
-        <v>4013</v>
+        <v>4026</v>
       </c>
     </row>
     <row r="745">
@@ -47018,7 +47018,7 @@
         <v>584.5</v>
       </c>
       <c r="T745" t="n">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="746">
@@ -47082,7 +47082,7 @@
         <v>9400</v>
       </c>
       <c r="T746" t="n">
-        <v>9923</v>
+        <v>9907</v>
       </c>
     </row>
     <row r="747">
@@ -47146,7 +47146,7 @@
         <v>1164</v>
       </c>
       <c r="T747" t="n">
-        <v>1459</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="748">
@@ -47326,7 +47326,7 @@
         <v>286.25</v>
       </c>
       <c r="T750" t="n">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="751">
@@ -47384,7 +47384,7 @@
         <v>135.125</v>
       </c>
       <c r="T751" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="752">
@@ -47512,7 +47512,7 @@
         <v>1998</v>
       </c>
       <c r="T753" t="n">
-        <v>1937</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="754">
@@ -47576,7 +47576,7 @@
         <v>215.75</v>
       </c>
       <c r="T754" t="n">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="755">
@@ -47768,7 +47768,7 @@
         <v>694.5</v>
       </c>
       <c r="T757" t="n">
-        <v>907</v>
+        <v>910</v>
       </c>
     </row>
     <row r="758">
@@ -47832,7 +47832,7 @@
         <v>957.5</v>
       </c>
       <c r="T758" t="n">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="759">
@@ -47960,7 +47960,7 @@
         <v>623.5</v>
       </c>
       <c r="T760" t="n">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="761">
@@ -48088,7 +48088,7 @@
         <v>6000</v>
       </c>
       <c r="T762" t="n">
-        <v>5110</v>
+        <v>5100</v>
       </c>
     </row>
     <row r="763">
@@ -48152,7 +48152,7 @@
         <v>634</v>
       </c>
       <c r="T763" t="n">
-        <v>837</v>
+        <v>841</v>
       </c>
     </row>
     <row r="764">
@@ -48408,7 +48408,7 @@
         <v>184.5</v>
       </c>
       <c r="T767" t="n">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="768">
@@ -48594,7 +48594,7 @@
         <v>915.5</v>
       </c>
       <c r="T770" t="n">
-        <v>969</v>
+        <v>971</v>
       </c>
     </row>
     <row r="771">
@@ -48722,7 +48722,7 @@
         <v>637</v>
       </c>
       <c r="T772" t="n">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="773">
@@ -49020,7 +49020,7 @@
         <v>820</v>
       </c>
       <c r="T777" t="n">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="778">
@@ -49148,7 +49148,7 @@
         <v>423.75</v>
       </c>
       <c r="T779" t="n">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="780">
@@ -49204,7 +49204,7 @@
         <v>0</v>
       </c>
       <c r="T780" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="781">
@@ -49268,7 +49268,7 @@
         <v>815</v>
       </c>
       <c r="T781" t="n">
-        <v>1116</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="782">
@@ -49396,7 +49396,7 @@
         <v>5012</v>
       </c>
       <c r="T783" t="n">
-        <v>5055</v>
+        <v>5043</v>
       </c>
     </row>
     <row r="784">
@@ -49460,7 +49460,7 @@
         <v>307.25</v>
       </c>
       <c r="T784" t="n">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="785">
@@ -49524,7 +49524,7 @@
         <v>272.25</v>
       </c>
       <c r="T785" t="n">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="786">
@@ -49652,7 +49652,7 @@
         <v>871</v>
       </c>
       <c r="T787" t="n">
-        <v>1155</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="788">
@@ -49780,7 +49780,7 @@
         <v>6620</v>
       </c>
       <c r="T789" t="n">
-        <v>5442</v>
+        <v>5426</v>
       </c>
     </row>
     <row r="790">
@@ -49844,7 +49844,7 @@
         <v>1008</v>
       </c>
       <c r="T790" t="n">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="791">
@@ -50036,7 +50036,7 @@
         <v>610.5</v>
       </c>
       <c r="T793" t="n">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="794">
@@ -50162,7 +50162,7 @@
         <v>430</v>
       </c>
       <c r="T795" t="n">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="796">
@@ -50220,7 +50220,7 @@
         <v>0</v>
       </c>
       <c r="T796" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="797">
@@ -50278,7 +50278,7 @@
         <v>200</v>
       </c>
       <c r="T797" t="n">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="798">
@@ -50342,7 +50342,7 @@
         <v>23.59375</v>
       </c>
       <c r="T798" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="799">
@@ -50406,7 +50406,7 @@
         <v>142</v>
       </c>
       <c r="T799" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="800">
@@ -50650,7 +50650,7 @@
         <v>219.625</v>
       </c>
       <c r="T803" t="n">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="804">
@@ -50778,7 +50778,7 @@
         <v>1195</v>
       </c>
       <c r="T805" t="n">
-        <v>1084</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="806">
@@ -50842,7 +50842,7 @@
         <v>216.125</v>
       </c>
       <c r="T806" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="807">
@@ -50970,7 +50970,7 @@
         <v>306.75</v>
       </c>
       <c r="T808" t="n">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="809">
@@ -51094,7 +51094,7 @@
         <v>708</v>
       </c>
       <c r="T810" t="n">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="811">
@@ -51280,7 +51280,7 @@
         <v>1075</v>
       </c>
       <c r="T813" t="n">
-        <v>1247</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="814">
@@ -51408,7 +51408,7 @@
         <v>7464</v>
       </c>
       <c r="T815" t="n">
-        <v>6952</v>
+        <v>6947</v>
       </c>
     </row>
     <row r="816">
@@ -51472,7 +51472,7 @@
         <v>192</v>
       </c>
       <c r="T816" t="n">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="817">
@@ -51536,7 +51536,7 @@
         <v>166.25</v>
       </c>
       <c r="T817" t="n">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="818">
@@ -51728,7 +51728,7 @@
         <v>22.890625</v>
       </c>
       <c r="T820" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="821">
@@ -51836,7 +51836,7 @@
         <v>0</v>
       </c>
       <c r="T822" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="823">
@@ -51964,7 +51964,7 @@
         <v>15.234375</v>
       </c>
       <c r="T824" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="825">
@@ -52028,7 +52028,7 @@
         <v>11</v>
       </c>
       <c r="T825" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="826">
@@ -52084,7 +52084,7 @@
         <v>0</v>
       </c>
       <c r="T826" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="827">
@@ -52192,7 +52192,7 @@
         <v>26.59375</v>
       </c>
       <c r="T828" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="829">
@@ -52320,7 +52320,7 @@
         <v>23.6875</v>
       </c>
       <c r="T830" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="831">
@@ -52384,7 +52384,7 @@
         <v>996.5</v>
       </c>
       <c r="T831" t="n">
-        <v>1122</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="832">
@@ -52448,7 +52448,7 @@
         <v>383.75</v>
       </c>
       <c r="T832" t="n">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="833">
@@ -52508,7 +52508,7 @@
         <v>250</v>
       </c>
       <c r="T833" t="n">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="834">
@@ -52810,7 +52810,7 @@
         <v>1.2255859375</v>
       </c>
       <c r="T838" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="839">
@@ -52874,7 +52874,7 @@
         <v>211.375</v>
       </c>
       <c r="T839" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="840">
@@ -52938,7 +52938,7 @@
         <v>598.5</v>
       </c>
       <c r="T840" t="n">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="841">
@@ -53002,7 +53002,7 @@
         <v>355.75</v>
       </c>
       <c r="T841" t="n">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="842">
@@ -53066,7 +53066,7 @@
         <v>2878</v>
       </c>
       <c r="T842" t="n">
-        <v>2873</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="843">
@@ -53130,7 +53130,7 @@
         <v>369.5</v>
       </c>
       <c r="T843" t="n">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="844">
@@ -53186,7 +53186,7 @@
         <v>1.349609375</v>
       </c>
       <c r="T844" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="845">
@@ -53240,7 +53240,7 @@
         <v>1</v>
       </c>
       <c r="T845" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="846">
@@ -53304,7 +53304,7 @@
         <v>1059</v>
       </c>
       <c r="T846" t="n">
-        <v>1340</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="847">
@@ -53432,7 +53432,7 @@
         <v>4148</v>
       </c>
       <c r="T848" t="n">
-        <v>4460</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="849">
@@ -53496,7 +53496,7 @@
         <v>620.5</v>
       </c>
       <c r="T849" t="n">
-        <v>863</v>
+        <v>865</v>
       </c>
     </row>
     <row r="850">
@@ -53560,7 +53560,7 @@
         <v>10840</v>
       </c>
       <c r="T850" t="n">
-        <v>12203</v>
+        <v>12180</v>
       </c>
     </row>
     <row r="851">
@@ -53624,7 +53624,7 @@
         <v>1178</v>
       </c>
       <c r="T851" t="n">
-        <v>1830</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="852">
@@ -53872,7 +53872,7 @@
         <v>383.75</v>
       </c>
       <c r="T855" t="n">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="856">
@@ -53936,7 +53936,7 @@
         <v>2106</v>
       </c>
       <c r="T856" t="n">
-        <v>2333</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="857">
@@ -54256,7 +54256,7 @@
         <v>1109</v>
       </c>
       <c r="T861" t="n">
-        <v>893</v>
+        <v>894</v>
       </c>
     </row>
     <row r="862">
@@ -54320,7 +54320,7 @@
         <v>136.625</v>
       </c>
       <c r="T862" t="n">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="863">
@@ -54448,7 +54448,7 @@
         <v>109.625</v>
       </c>
       <c r="T864" t="n">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="865">
@@ -54512,7 +54512,7 @@
         <v>6428</v>
       </c>
       <c r="T865" t="n">
-        <v>5969</v>
+        <v>5959</v>
       </c>
     </row>
     <row r="866">
@@ -54576,7 +54576,7 @@
         <v>754</v>
       </c>
       <c r="T866" t="n">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="867">
@@ -54768,7 +54768,7 @@
         <v>448</v>
       </c>
       <c r="T869" t="n">
-        <v>554</v>
+        <v>550</v>
       </c>
     </row>
     <row r="870">
@@ -54832,7 +54832,7 @@
         <v>207.25</v>
       </c>
       <c r="T870" t="n">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="871">
@@ -54890,7 +54890,7 @@
         <v>12.90625</v>
       </c>
       <c r="T871" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="872">
@@ -55018,7 +55018,7 @@
         <v>939</v>
       </c>
       <c r="T873" t="n">
-        <v>1121</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="874">
@@ -55082,7 +55082,7 @@
         <v>99.6875</v>
       </c>
       <c r="T874" t="n">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="875">
@@ -55146,7 +55146,7 @@
         <v>703</v>
       </c>
       <c r="T875" t="n">
-        <v>721</v>
+        <v>716</v>
       </c>
     </row>
     <row r="876">
@@ -55326,7 +55326,7 @@
         <v>0</v>
       </c>
       <c r="T878" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="879">
@@ -55444,7 +55444,7 @@
         <v>915.5</v>
       </c>
       <c r="T880" t="n">
-        <v>1038</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="881">
@@ -55694,7 +55694,7 @@
         <v>879</v>
       </c>
       <c r="T884" t="n">
-        <v>1310</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="885">
@@ -55822,7 +55822,7 @@
         <v>5396</v>
       </c>
       <c r="T886" t="n">
-        <v>5999</v>
+        <v>6023</v>
       </c>
     </row>
     <row r="887">
@@ -55886,7 +55886,7 @@
         <v>416.75</v>
       </c>
       <c r="T887" t="n">
-        <v>665</v>
+        <v>667</v>
       </c>
     </row>
     <row r="888">
@@ -56078,7 +56078,7 @@
         <v>929.5</v>
       </c>
       <c r="T890" t="n">
-        <v>1367</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="891">
@@ -56270,7 +56270,7 @@
         <v>1253</v>
       </c>
       <c r="T893" t="n">
-        <v>1597</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="894">
@@ -56588,7 +56588,7 @@
         <v>436.75</v>
       </c>
       <c r="T898" t="n">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="899">
@@ -56646,7 +56646,7 @@
         <v>0</v>
       </c>
       <c r="T899" t="n">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="900">
@@ -57074,7 +57074,7 @@
         <v>220.5</v>
       </c>
       <c r="T906" t="n">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="907">
@@ -57202,7 +57202,7 @@
         <v>1363</v>
       </c>
       <c r="T908" t="n">
-        <v>1349</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="909">
@@ -57266,7 +57266,7 @@
         <v>221.625</v>
       </c>
       <c r="T909" t="n">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="910">
@@ -57394,7 +57394,7 @@
         <v>369</v>
       </c>
       <c r="T911" t="n">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="912">
@@ -57456,7 +57456,7 @@
         <v>12.671875</v>
       </c>
       <c r="T912" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="913">
@@ -57520,7 +57520,7 @@
         <v>779</v>
       </c>
       <c r="T913" t="n">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="914">
@@ -57834,7 +57834,7 @@
         <v>8776</v>
       </c>
       <c r="T918" t="n">
-        <v>8918</v>
+        <v>8927</v>
       </c>
     </row>
     <row r="919">
@@ -57898,7 +57898,7 @@
         <v>201</v>
       </c>
       <c r="T919" t="n">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="920">
@@ -57962,7 +57962,7 @@
         <v>191.375</v>
       </c>
       <c r="T920" t="n">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="921">
@@ -58090,7 +58090,7 @@
         <v>123.75</v>
       </c>
       <c r="T922" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="923">
@@ -58402,7 +58402,7 @@
         <v>0</v>
       </c>
       <c r="T927" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="928">
@@ -58512,7 +58512,7 @@
         <v>1</v>
       </c>
       <c r="T929" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="930">
@@ -58576,7 +58576,7 @@
         <v>194.75</v>
       </c>
       <c r="T930" t="n">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="931">
@@ -58640,7 +58640,7 @@
         <v>75.6875</v>
       </c>
       <c r="T931" t="n">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="932">
@@ -58704,7 +58704,7 @@
         <v>1312</v>
       </c>
       <c r="T932" t="n">
-        <v>2099</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="933">
@@ -58768,7 +58768,7 @@
         <v>405.5</v>
       </c>
       <c r="T933" t="n">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="934">
@@ -58828,7 +58828,7 @@
         <v>457.75</v>
       </c>
       <c r="T934" t="n">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="935">
@@ -58892,7 +58892,7 @@
         <v>100</v>
       </c>
       <c r="T935" t="n">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="936">
@@ -58956,7 +58956,7 @@
         <v>52.5625</v>
       </c>
       <c r="T936" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="937">
@@ -59020,7 +59020,7 @@
         <v>233.5</v>
       </c>
       <c r="T937" t="n">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="938">
@@ -59132,7 +59132,7 @@
         <v>1.2255859375</v>
       </c>
       <c r="T939" t="n">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="940">
@@ -59196,7 +59196,7 @@
         <v>258</v>
       </c>
       <c r="T940" t="n">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="941">
@@ -59260,7 +59260,7 @@
         <v>759.5</v>
       </c>
       <c r="T941" t="n">
-        <v>737</v>
+        <v>733</v>
       </c>
     </row>
     <row r="942">
@@ -59324,7 +59324,7 @@
         <v>349.75</v>
       </c>
       <c r="T942" t="n">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>